<commit_message>
REQ: force delete on cmd-line
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="16"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6048" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6055" uniqueCount="957">
   <si>
     <t>SVN</t>
   </si>
@@ -3083,6 +3083,18 @@
   </si>
   <si>
     <t>MediaStore</t>
+  </si>
+  <si>
+    <t>no use</t>
+  </si>
+  <si>
+    <t>Force delete</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Do not ask for confirmation to delete the previously generated data</t>
   </si>
 </sst>
 </file>
@@ -35868,7 +35880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -36122,10 +36134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D51"/>
+  <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36134,12 +36146,12 @@
     <col min="3" max="3" width="107.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:5">
       <c r="D1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:5">
       <c r="B3" s="16" t="s">
         <v>338</v>
       </c>
@@ -36150,7 +36162,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:5">
       <c r="B4" s="7" t="s">
         <v>69</v>
       </c>
@@ -36161,7 +36173,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:5">
       <c r="B5" s="7" t="s">
         <v>70</v>
       </c>
@@ -36172,19 +36184,25 @@
         <v>802</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="B6" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="E6" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="E7" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
       <c r="B8" s="7" t="s">
         <v>75</v>
       </c>
@@ -36195,7 +36213,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:5">
       <c r="B9" s="17" t="s">
         <v>376</v>
       </c>
@@ -36203,7 +36221,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:5">
       <c r="B10" s="7" t="s">
         <v>0</v>
       </c>
@@ -36214,7 +36232,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:5">
       <c r="B11" s="7" t="s">
         <v>92</v>
       </c>
@@ -36225,7 +36243,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:5">
       <c r="B12" s="17" t="s">
         <v>340</v>
       </c>
@@ -36236,7 +36254,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:5">
       <c r="B13" s="19" t="s">
         <v>380</v>
       </c>
@@ -36244,7 +36262,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:5">
       <c r="B14" s="19" t="s">
         <v>381</v>
       </c>
@@ -36252,7 +36270,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:5">
       <c r="B15" s="19" t="s">
         <v>408</v>
       </c>
@@ -36260,7 +36278,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:5">
       <c r="B16" s="7" t="s">
         <v>382</v>
       </c>
@@ -36271,7 +36289,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:5">
       <c r="B17" s="7" t="s">
         <v>384</v>
       </c>
@@ -36282,7 +36300,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:5">
       <c r="B18" s="7" t="s">
         <v>343</v>
       </c>
@@ -36293,7 +36311,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:5">
       <c r="B19" s="7" t="s">
         <v>341</v>
       </c>
@@ -36304,7 +36322,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:5">
       <c r="B20" s="7" t="s">
         <v>359</v>
       </c>
@@ -36315,7 +36333,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:5">
       <c r="B21" s="7" t="s">
         <v>364</v>
       </c>
@@ -36325,8 +36343,11 @@
       <c r="D21" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="E21" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22" s="7" t="s">
         <v>374</v>
       </c>
@@ -36336,8 +36357,11 @@
       <c r="D22" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
+      <c r="E22" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="24" t="s">
         <v>413</v>
       </c>
@@ -36346,7 +36370,7 @@
       </c>
       <c r="D23" s="23"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:5">
       <c r="B24" s="29" t="s">
         <v>798</v>
       </c>
@@ -36354,7 +36378,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:5">
       <c r="B25" s="29" t="s">
         <v>799</v>
       </c>
@@ -36362,35 +36386,42 @@
         <v>800</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="30" t="s">
+    <row r="26" spans="2:5" s="32" customFormat="1">
+      <c r="B26" s="29" t="s">
+        <v>954</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>955</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="30" t="s">
         <v>795</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="30" t="s">
+    <row r="28" spans="2:5">
+      <c r="B28" s="30" t="s">
         <v>813</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C28" s="31" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:5">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:5">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:5">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
@@ -36398,13 +36429,13 @@
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+    <row r="34" spans="2:3">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
+      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="7"/>
@@ -36412,19 +36443,19 @@
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" spans="2:3">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+    <row r="40" spans="2:3">
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
+      <c r="C42" s="7"/>
     </row>
     <row r="43" spans="2:3">
       <c r="B43" s="7"/>
@@ -36432,15 +36463,15 @@
     </row>
     <row r="44" spans="2:3">
       <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
+    <row r="46" spans="2:3">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
     </row>
     <row r="48" spans="2:3">
       <c r="B48" s="7"/>
@@ -36448,15 +36479,19 @@
     </row>
     <row r="49" spans="2:3">
       <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
+      <c r="C49" s="7"/>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" spans="2:3">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ENH: entity instance in handlers should contain its original ID (the one written in Excel) - preparation for Kanban
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="12"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7515" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7515" uniqueCount="1095">
   <si>
     <t>SVN</t>
   </si>
@@ -3508,20 +3508,23 @@
   <si>
     <t>2012-09-22 08:13:12</t>
   </si>
+  <si>
+    <t>_not-used-id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_ &quot;₪&quot;\ * #,##0_ ;_ &quot;₪&quot;\ * \-#,##0_ ;_ &quot;₪&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ &quot;₪&quot;\ * #,##0.00_ ;_ &quot;₪&quot;\ * \-#,##0.00_ ;_ &quot;₪&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_ &quot;₪&quot;\ * #,##0_ ;_ &quot;₪&quot;\ * \-#,##0_ ;_ &quot;₪&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="_ &quot;₪&quot;\ * #,##0.00_ ;_ &quot;₪&quot;\ * \-#,##0.00_ ;_ &quot;₪&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -3674,28 +3677,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
@@ -7301,7 +7304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I721"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -19033,9 +19036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H336"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F339" sqref="F339"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -19051,7 +19052,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="32" t="s">
-        <v>10</v>
+        <v>1094</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
REQ: remove RBLI assignees -> it generates too many void e-mails
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="13"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7957" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7740" uniqueCount="1114">
   <si>
     <t>SVN</t>
   </si>
@@ -14401,7 +14401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+    <sheetView topLeftCell="A207" workbookViewId="0">
       <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
@@ -19022,8 +19022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L336"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19096,7 +19096,7 @@
         <v>320</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>309</v>
+        <v>15</v>
       </c>
       <c r="G2" s="32">
         <v>4</v>
@@ -19130,9 +19130,6 @@
       <c r="E3" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G3" s="32">
         <v>6</v>
       </c>
@@ -19165,9 +19162,6 @@
       <c r="E4" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G4" s="32">
         <v>10</v>
       </c>
@@ -19200,9 +19194,6 @@
       <c r="E5" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G5" s="32">
         <v>6</v>
       </c>
@@ -19235,9 +19226,6 @@
       <c r="E6" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G6" s="32">
         <v>2</v>
       </c>
@@ -19270,9 +19258,6 @@
       <c r="E7" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F7" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G7" s="32">
         <v>8</v>
       </c>
@@ -19305,9 +19290,6 @@
       <c r="E8" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G8" s="32">
         <v>6</v>
       </c>
@@ -19340,9 +19322,6 @@
       <c r="E9" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G9" s="32">
         <v>8</v>
       </c>
@@ -19375,9 +19354,6 @@
       <c r="E10" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G10" s="32">
         <v>2</v>
       </c>
@@ -19410,9 +19386,6 @@
       <c r="E11" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F11" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G11" s="32">
         <v>4</v>
       </c>
@@ -19445,9 +19418,6 @@
       <c r="E12" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F12" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G12" s="32">
         <v>2</v>
       </c>
@@ -19480,9 +19450,6 @@
       <c r="E13" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G13" s="32">
         <v>6</v>
       </c>
@@ -19518,9 +19485,6 @@
       <c r="E14" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G14" s="32">
         <v>8</v>
       </c>
@@ -19553,9 +19517,6 @@
       <c r="E15" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F15" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G15" s="32">
         <v>6</v>
       </c>
@@ -19588,9 +19549,6 @@
       <c r="E16" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F16" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G16" s="32">
         <v>2</v>
       </c>
@@ -19623,9 +19581,6 @@
       <c r="E17" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F17" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G17" s="32">
         <v>2</v>
       </c>
@@ -19658,9 +19613,6 @@
       <c r="E18" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F18" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G18" s="32">
         <v>6</v>
       </c>
@@ -19693,9 +19645,6 @@
       <c r="E19" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F19" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G19" s="32">
         <v>2</v>
       </c>
@@ -19728,9 +19677,6 @@
       <c r="E20" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F20" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G20" s="32">
         <v>2</v>
       </c>
@@ -19763,9 +19709,6 @@
       <c r="E21" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G21" s="32">
         <v>2</v>
       </c>
@@ -19798,9 +19741,6 @@
       <c r="E22" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F22" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G22" s="32">
         <v>2</v>
       </c>
@@ -19833,9 +19773,6 @@
       <c r="E23" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F23" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G23" s="32">
         <v>6</v>
       </c>
@@ -19868,9 +19805,6 @@
       <c r="E24" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F24" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G24" s="32">
         <v>2</v>
       </c>
@@ -19903,9 +19837,6 @@
       <c r="E25" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F25" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G25" s="32">
         <v>2</v>
       </c>
@@ -19941,9 +19872,6 @@
       <c r="E26" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F26" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G26" s="32">
         <v>2</v>
       </c>
@@ -19976,9 +19904,6 @@
       <c r="E27" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F27" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G27" s="32">
         <v>6</v>
       </c>
@@ -20011,9 +19936,6 @@
       <c r="E28" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F28" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G28" s="32">
         <v>6</v>
       </c>
@@ -20046,9 +19968,6 @@
       <c r="E29" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F29" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G29" s="32">
         <v>2</v>
       </c>
@@ -20081,9 +20000,6 @@
       <c r="E30" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F30" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G30" s="32">
         <v>8</v>
       </c>
@@ -20116,9 +20032,6 @@
       <c r="E31" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F31" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G31" s="32">
         <v>2</v>
       </c>
@@ -20151,9 +20064,6 @@
       <c r="E32" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F32" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G32" s="32">
         <v>6</v>
       </c>
@@ -20186,9 +20096,6 @@
       <c r="E33" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F33" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G33" s="32">
         <v>2</v>
       </c>
@@ -20221,9 +20128,6 @@
       <c r="E34" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F34" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G34" s="32">
         <v>2</v>
       </c>
@@ -20256,9 +20160,6 @@
       <c r="E35" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F35" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G35" s="32">
         <v>6</v>
       </c>
@@ -20291,9 +20192,6 @@
       <c r="E36" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F36" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G36" s="32">
         <v>8</v>
       </c>
@@ -20326,9 +20224,6 @@
       <c r="E37" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F37" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G37" s="32">
         <v>2</v>
       </c>
@@ -20361,9 +20256,6 @@
       <c r="E38" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F38" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G38" s="32">
         <v>4</v>
       </c>
@@ -20396,9 +20288,6 @@
       <c r="E39" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F39" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G39" s="32">
         <v>8</v>
       </c>
@@ -20431,9 +20320,6 @@
       <c r="E40" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F40" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G40" s="32">
         <v>2</v>
       </c>
@@ -20466,9 +20352,6 @@
       <c r="E41" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F41" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G41" s="32">
         <v>6</v>
       </c>
@@ -20501,9 +20384,6 @@
       <c r="E42" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F42" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G42" s="32">
         <v>2</v>
       </c>
@@ -20536,9 +20416,6 @@
       <c r="E43" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F43" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G43" s="32">
         <v>2</v>
       </c>
@@ -20571,9 +20448,6 @@
       <c r="E44" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F44" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G44" s="32">
         <v>2</v>
       </c>
@@ -20606,9 +20480,6 @@
       <c r="E45" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F45" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G45" s="32">
         <v>8</v>
       </c>
@@ -20641,9 +20512,6 @@
       <c r="E46" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F46" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G46" s="32">
         <v>8</v>
       </c>
@@ -20676,9 +20544,6 @@
       <c r="E47" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F47" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G47" s="32">
         <v>2</v>
       </c>
@@ -20711,9 +20576,6 @@
       <c r="E48" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F48" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G48" s="32">
         <v>8</v>
       </c>
@@ -20746,9 +20608,6 @@
       <c r="E49" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F49" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G49" s="32">
         <v>6</v>
       </c>
@@ -20781,9 +20640,6 @@
       <c r="E50" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F50" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G50" s="32">
         <v>4</v>
       </c>
@@ -20816,9 +20672,6 @@
       <c r="E51" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F51" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G51" s="32">
         <v>2</v>
       </c>
@@ -20851,9 +20704,6 @@
       <c r="E52" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F52" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G52" s="32">
         <v>6</v>
       </c>
@@ -20886,9 +20736,6 @@
       <c r="E53" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F53" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G53" s="32">
         <v>6</v>
       </c>
@@ -20921,9 +20768,6 @@
       <c r="E54" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F54" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G54" s="32">
         <v>6</v>
       </c>
@@ -20956,9 +20800,6 @@
       <c r="E55" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F55" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G55" s="32">
         <v>2</v>
       </c>
@@ -20991,9 +20832,6 @@
       <c r="E56" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F56" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G56" s="32">
         <v>2</v>
       </c>
@@ -21026,9 +20864,6 @@
       <c r="E57" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F57" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G57" s="32">
         <v>6</v>
       </c>
@@ -21061,9 +20896,6 @@
       <c r="E58" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F58" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G58" s="32">
         <v>2</v>
       </c>
@@ -21096,9 +20928,6 @@
       <c r="E59" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F59" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G59" s="32">
         <v>2</v>
       </c>
@@ -21131,9 +20960,6 @@
       <c r="E60" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F60" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G60" s="32">
         <v>4</v>
       </c>
@@ -21166,9 +20992,6 @@
       <c r="E61" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F61" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G61" s="32">
         <v>2</v>
       </c>
@@ -21201,9 +21024,6 @@
       <c r="E62" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F62" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G62" s="32">
         <v>6</v>
       </c>
@@ -21236,9 +21056,6 @@
       <c r="E63" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F63" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G63" s="32">
         <v>4</v>
       </c>
@@ -21271,9 +21088,6 @@
       <c r="E64" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F64" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G64" s="32">
         <v>6</v>
       </c>
@@ -21306,9 +21120,6 @@
       <c r="E65" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F65" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G65" s="32">
         <v>2</v>
       </c>
@@ -21341,9 +21152,6 @@
       <c r="E66" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F66" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G66" s="32">
         <v>8</v>
       </c>
@@ -21376,9 +21184,6 @@
       <c r="E67" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F67" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G67" s="32">
         <v>2</v>
       </c>
@@ -21411,9 +21216,6 @@
       <c r="E68" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F68" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G68" s="32">
         <v>2</v>
       </c>
@@ -21446,9 +21248,6 @@
       <c r="E69" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F69" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G69" s="32">
         <v>2</v>
       </c>
@@ -21481,9 +21280,6 @@
       <c r="E70" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F70" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G70" s="32">
         <v>6</v>
       </c>
@@ -21516,9 +21312,6 @@
       <c r="E71" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F71" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G71" s="32">
         <v>6</v>
       </c>
@@ -21551,9 +21344,6 @@
       <c r="E72" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F72" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G72" s="32">
         <v>6</v>
       </c>
@@ -21586,9 +21376,6 @@
       <c r="E73" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F73" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G73" s="32">
         <v>2</v>
       </c>
@@ -21621,9 +21408,6 @@
       <c r="E74" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F74" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G74" s="32">
         <v>2</v>
       </c>
@@ -21656,9 +21440,6 @@
       <c r="E75" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F75" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G75" s="32">
         <v>6</v>
       </c>
@@ -21691,9 +21472,6 @@
       <c r="E76" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F76" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G76" s="32">
         <v>2</v>
       </c>
@@ -21726,9 +21504,6 @@
       <c r="E77" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F77" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G77" s="32">
         <v>2</v>
       </c>
@@ -21761,9 +21536,6 @@
       <c r="E78" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F78" s="32" t="s">
-        <v>319</v>
-      </c>
       <c r="G78" s="32">
         <v>2</v>
       </c>
@@ -21796,9 +21568,6 @@
       <c r="E79" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F79" s="32" t="s">
-        <v>313</v>
-      </c>
       <c r="G79" s="32">
         <v>2</v>
       </c>
@@ -21831,9 +21600,6 @@
       <c r="E80" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F80" s="32" t="s">
-        <v>310</v>
-      </c>
       <c r="G80" s="32">
         <v>6</v>
       </c>
@@ -21866,9 +21632,6 @@
       <c r="E81" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F81" s="32" t="s">
-        <v>317</v>
-      </c>
       <c r="G81" s="32">
         <v>2</v>
       </c>
@@ -21901,9 +21664,6 @@
       <c r="E82" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F82" s="32" t="s">
-        <v>314</v>
-      </c>
       <c r="G82" s="32">
         <v>12</v>
       </c>
@@ -21936,9 +21696,6 @@
       <c r="E83" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F83" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G83" s="32">
         <v>2</v>
       </c>
@@ -21971,9 +21728,6 @@
       <c r="E84" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F84" s="32" t="s">
-        <v>318</v>
-      </c>
       <c r="G84" s="32">
         <v>2</v>
       </c>
@@ -22006,9 +21760,6 @@
       <c r="E85" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F85" s="32" t="s">
-        <v>315</v>
-      </c>
       <c r="G85" s="32">
         <v>6</v>
       </c>
@@ -22041,9 +21792,6 @@
       <c r="E86" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F86" s="32" t="s">
-        <v>309</v>
-      </c>
       <c r="G86" s="32">
         <v>4</v>
       </c>
@@ -22076,9 +21824,6 @@
       <c r="E87" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="F87" s="32" t="s">
-        <v>316</v>
-      </c>
       <c r="G87" s="32">
         <v>6</v>
       </c>
@@ -22111,9 +21856,6 @@
       <c r="E88" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="F88" s="32" t="s">
-        <v>312</v>
-      </c>
       <c r="G88" s="32">
         <v>2</v>
       </c>
@@ -22146,9 +21888,6 @@
       <c r="E89" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F89" s="32" t="s">
-        <v>311</v>
-      </c>
       <c r="G89" s="32">
         <v>2</v>
       </c>
@@ -22181,9 +21920,6 @@
       <c r="E90" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F90" s="32" t="s">
-        <v>15</v>
-      </c>
       <c r="G90" s="32">
         <v>6</v>
       </c>
@@ -22583,9 +22319,6 @@
       <c r="E122" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F122" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G122" s="41">
         <v>3</v>
       </c>
@@ -22618,9 +22351,6 @@
       <c r="E123" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F123" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G123" s="41" t="s">
         <v>937</v>
       </c>
@@ -22653,9 +22383,6 @@
       <c r="E124" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F124" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G124" s="41" t="s">
         <v>936</v>
       </c>
@@ -22688,9 +22415,6 @@
       <c r="E125" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F125" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G125" s="6">
         <v>3</v>
       </c>
@@ -22723,9 +22447,6 @@
       <c r="E126" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F126" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G126" s="6">
         <v>1</v>
       </c>
@@ -22758,9 +22479,6 @@
       <c r="E127" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F127" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G127" s="6">
         <v>5</v>
       </c>
@@ -22793,9 +22511,6 @@
       <c r="E128" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F128" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G128" s="6">
         <v>3</v>
       </c>
@@ -22828,9 +22543,6 @@
       <c r="E129" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F129" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G129" s="6">
         <v>5</v>
       </c>
@@ -22863,9 +22575,6 @@
       <c r="E130" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F130" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G130" s="6">
         <v>1</v>
       </c>
@@ -22898,9 +22607,6 @@
       <c r="E131" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F131" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G131" s="6">
         <v>3</v>
       </c>
@@ -22933,9 +22639,6 @@
       <c r="E132" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F132" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G132" s="6">
         <v>3</v>
       </c>
@@ -22968,9 +22671,6 @@
       <c r="E133" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F133" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G133" s="6">
         <v>3</v>
       </c>
@@ -23003,9 +22703,6 @@
       <c r="E134" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F134" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G134" s="6">
         <v>3</v>
       </c>
@@ -23038,9 +22735,6 @@
       <c r="E135" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F135" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G135" s="6">
         <v>3</v>
       </c>
@@ -23073,9 +22767,6 @@
       <c r="E136" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F136" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G136" s="6">
         <v>3</v>
       </c>
@@ -23108,9 +22799,6 @@
       <c r="E137" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F137" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G137" s="6">
         <v>3</v>
       </c>
@@ -23143,9 +22831,6 @@
       <c r="E138" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F138" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G138" s="6">
         <v>1</v>
       </c>
@@ -23178,9 +22863,6 @@
       <c r="E139" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F139" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G139" s="6">
         <v>3</v>
       </c>
@@ -23213,9 +22895,6 @@
       <c r="E140" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F140" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G140" s="6">
         <v>3</v>
       </c>
@@ -23248,9 +22927,6 @@
       <c r="E141" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F141" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G141" s="6">
         <v>1</v>
       </c>
@@ -23283,9 +22959,6 @@
       <c r="E142" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F142" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G142" s="6">
         <v>1</v>
       </c>
@@ -23318,9 +22991,6 @@
       <c r="E143" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F143" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G143" s="6">
         <v>2</v>
       </c>
@@ -23353,9 +23023,6 @@
       <c r="E144" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F144" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G144" s="6">
         <v>3</v>
       </c>
@@ -23388,9 +23055,6 @@
       <c r="E145" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F145" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G145" s="6">
         <v>3</v>
       </c>
@@ -23423,9 +23087,6 @@
       <c r="E146" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F146" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G146" s="6">
         <v>2</v>
       </c>
@@ -23458,9 +23119,6 @@
       <c r="E147" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F147" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G147" s="6">
         <v>3</v>
       </c>
@@ -23493,9 +23151,6 @@
       <c r="E148" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F148" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G148" s="6">
         <v>3</v>
       </c>
@@ -23528,9 +23183,6 @@
       <c r="E149" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F149" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G149" s="6">
         <v>3</v>
       </c>
@@ -23563,9 +23215,6 @@
       <c r="E150" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F150" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G150" s="6">
         <v>2</v>
       </c>
@@ -23598,9 +23247,6 @@
       <c r="E151" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F151" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G151" s="6">
         <v>2</v>
       </c>
@@ -23633,9 +23279,6 @@
       <c r="E152" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F152" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G152" s="6">
         <v>2</v>
       </c>
@@ -23668,9 +23311,6 @@
       <c r="E153" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F153" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G153" s="6">
         <v>2</v>
       </c>
@@ -23703,9 +23343,6 @@
       <c r="E154" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F154" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G154" s="6">
         <v>2</v>
       </c>
@@ -23738,9 +23375,6 @@
       <c r="E155" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F155" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G155" s="6">
         <v>1</v>
       </c>
@@ -23773,9 +23407,6 @@
       <c r="E156" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F156" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G156" s="6">
         <v>1</v>
       </c>
@@ -23808,9 +23439,6 @@
       <c r="E157" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F157" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G157" s="6">
         <v>5</v>
       </c>
@@ -23843,9 +23471,6 @@
       <c r="E158" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F158" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G158" s="6">
         <v>3</v>
       </c>
@@ -23881,9 +23506,6 @@
       <c r="E159" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F159" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G159" s="6">
         <v>1</v>
       </c>
@@ -23916,9 +23538,6 @@
       <c r="E160" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F160" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G160" s="6">
         <v>3</v>
       </c>
@@ -23951,9 +23570,6 @@
       <c r="E161" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F161" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G161" s="6">
         <v>2</v>
       </c>
@@ -23986,9 +23602,6 @@
       <c r="E162" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F162" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G162" s="6">
         <v>1</v>
       </c>
@@ -24021,9 +23634,6 @@
       <c r="E163" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F163" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G163" s="6">
         <v>1</v>
       </c>
@@ -24056,9 +23666,6 @@
       <c r="E164" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F164" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G164" s="6">
         <v>3</v>
       </c>
@@ -24091,9 +23698,6 @@
       <c r="E165" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F165" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G165" s="6">
         <v>3</v>
       </c>
@@ -24126,9 +23730,6 @@
       <c r="E166" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F166" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G166" s="6">
         <v>3</v>
       </c>
@@ -24161,9 +23762,6 @@
       <c r="E167" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F167" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G167" s="6">
         <v>3</v>
       </c>
@@ -24196,9 +23794,6 @@
       <c r="E168" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F168" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G168" s="6">
         <v>3</v>
       </c>
@@ -24231,9 +23826,6 @@
       <c r="E169" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F169" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G169" s="6">
         <v>3</v>
       </c>
@@ -24266,9 +23858,6 @@
       <c r="E170" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F170" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G170" s="6">
         <v>3</v>
       </c>
@@ -24301,9 +23890,6 @@
       <c r="E171" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F171" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G171" s="6">
         <v>3</v>
       </c>
@@ -24336,9 +23922,6 @@
       <c r="E172" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F172" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G172" s="6">
         <v>3</v>
       </c>
@@ -24371,9 +23954,6 @@
       <c r="E173" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F173" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G173" s="6">
         <v>3</v>
       </c>
@@ -24406,9 +23986,6 @@
       <c r="E174" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F174" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G174" s="6">
         <v>2</v>
       </c>
@@ -24441,9 +24018,6 @@
       <c r="E175" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F175" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G175" s="6">
         <v>3</v>
       </c>
@@ -24476,9 +24050,6 @@
       <c r="E176" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F176" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G176" s="6">
         <v>3</v>
       </c>
@@ -24511,9 +24082,6 @@
       <c r="E177" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F177" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G177" s="6">
         <v>1</v>
       </c>
@@ -24546,9 +24114,6 @@
       <c r="E178" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F178" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G178" s="6">
         <v>1</v>
       </c>
@@ -24581,9 +24146,6 @@
       <c r="E179" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F179" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G179" s="6">
         <v>1</v>
       </c>
@@ -24616,9 +24178,6 @@
       <c r="E180" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F180" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G180" s="6">
         <v>3</v>
       </c>
@@ -24651,9 +24210,6 @@
       <c r="E181" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F181" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G181" s="6">
         <v>3</v>
       </c>
@@ -24686,9 +24242,6 @@
       <c r="E182" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F182" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G182" s="6">
         <v>3</v>
       </c>
@@ -24721,9 +24274,6 @@
       <c r="E183" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F183" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G183" s="6">
         <v>3</v>
       </c>
@@ -24756,9 +24306,6 @@
       <c r="E184" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F184" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G184" s="6">
         <v>3</v>
       </c>
@@ -24791,9 +24338,6 @@
       <c r="E185" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F185" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G185" s="6">
         <v>3</v>
       </c>
@@ -24826,9 +24370,6 @@
       <c r="E186" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F186" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G186" s="6">
         <v>4</v>
       </c>
@@ -24861,9 +24402,6 @@
       <c r="E187" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F187" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G187" s="6">
         <v>2</v>
       </c>
@@ -24896,9 +24434,6 @@
       <c r="E188" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F188" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G188" s="6">
         <v>3</v>
       </c>
@@ -24931,9 +24466,6 @@
       <c r="E189" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F189" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G189" s="6">
         <v>3</v>
       </c>
@@ -24966,9 +24498,6 @@
       <c r="E190" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F190" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G190" s="6">
         <v>3</v>
       </c>
@@ -25001,9 +24530,6 @@
       <c r="E191" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F191" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G191" s="6">
         <v>1</v>
       </c>
@@ -25036,9 +24562,6 @@
       <c r="E192" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F192" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G192" s="6">
         <v>1</v>
       </c>
@@ -25071,9 +24594,6 @@
       <c r="E193" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F193" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G193" s="6">
         <v>3</v>
       </c>
@@ -25109,9 +24629,6 @@
       <c r="E194" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F194" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G194" s="6">
         <v>3</v>
       </c>
@@ -25144,9 +24661,6 @@
       <c r="E195" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F195" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G195" s="6">
         <v>1</v>
       </c>
@@ -25179,9 +24693,6 @@
       <c r="E196" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F196" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G196" s="6">
         <v>3</v>
       </c>
@@ -25214,9 +24725,6 @@
       <c r="E197" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F197" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G197" s="6">
         <v>2</v>
       </c>
@@ -25249,9 +24757,6 @@
       <c r="E198" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F198" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G198" s="6">
         <v>1</v>
       </c>
@@ -25284,9 +24789,6 @@
       <c r="E199" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F199" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G199" s="6">
         <v>1</v>
       </c>
@@ -25319,9 +24821,6 @@
       <c r="E200" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F200" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G200" s="6">
         <v>3</v>
       </c>
@@ -25354,9 +24853,6 @@
       <c r="E201" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F201" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G201" s="6">
         <v>3</v>
       </c>
@@ -25389,9 +24885,6 @@
       <c r="E202" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F202" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G202" s="6">
         <v>3</v>
       </c>
@@ -25424,9 +24917,6 @@
       <c r="E203" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F203" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G203" s="6">
         <v>3</v>
       </c>
@@ -25459,9 +24949,6 @@
       <c r="E204" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F204" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G204" s="6">
         <v>3</v>
       </c>
@@ -25494,9 +24981,6 @@
       <c r="E205" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F205" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G205" s="6">
         <v>3</v>
       </c>
@@ -25529,9 +25013,6 @@
       <c r="E206" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F206" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G206" s="6">
         <v>3</v>
       </c>
@@ -25564,9 +25045,6 @@
       <c r="E207" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F207" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G207" s="6">
         <v>3</v>
       </c>
@@ -25599,9 +25077,6 @@
       <c r="E208" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F208" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G208" s="6">
         <v>3</v>
       </c>
@@ -25634,9 +25109,6 @@
       <c r="E209" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F209" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G209" s="6">
         <v>3</v>
       </c>
@@ -25669,9 +25141,6 @@
       <c r="E210" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F210" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G210" s="6">
         <v>2</v>
       </c>
@@ -25704,9 +25173,6 @@
       <c r="E211" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F211" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G211" s="6">
         <v>3</v>
       </c>
@@ -25739,9 +25205,6 @@
       <c r="E212" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F212" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G212" s="6">
         <v>3</v>
       </c>
@@ -25774,9 +25237,6 @@
       <c r="E213" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F213" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G213" s="6">
         <v>1</v>
       </c>
@@ -25812,9 +25272,6 @@
       <c r="E214" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F214" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G214" s="6">
         <v>2</v>
       </c>
@@ -25847,9 +25304,6 @@
       <c r="E215" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F215" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G215" s="6">
         <v>2</v>
       </c>
@@ -25882,9 +25336,6 @@
       <c r="E216" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F216" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G216" s="6">
         <v>3</v>
       </c>
@@ -25917,9 +25368,6 @@
       <c r="E217" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F217" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G217" s="6">
         <v>3</v>
       </c>
@@ -25952,9 +25400,6 @@
       <c r="E218" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F218" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G218" s="6">
         <v>2</v>
       </c>
@@ -25987,9 +25432,6 @@
       <c r="E219" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F219" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G219" s="6">
         <v>3</v>
       </c>
@@ -26022,9 +25464,6 @@
       <c r="E220" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F220" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G220" s="6">
         <v>3</v>
       </c>
@@ -26057,9 +25496,6 @@
       <c r="E221" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F221" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G221" s="6">
         <v>3</v>
       </c>
@@ -26092,9 +25528,6 @@
       <c r="E222" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F222" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G222" s="6">
         <v>5</v>
       </c>
@@ -26127,9 +25560,6 @@
       <c r="E223" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F223" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G223" s="6">
         <v>4</v>
       </c>
@@ -26162,9 +25592,6 @@
       <c r="E224" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F224" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G224" s="6">
         <v>3</v>
       </c>
@@ -26197,9 +25624,6 @@
       <c r="E225" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F225" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G225" s="6">
         <v>3</v>
       </c>
@@ -26232,9 +25656,6 @@
       <c r="E226" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F226" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G226" s="6">
         <v>3</v>
       </c>
@@ -26267,9 +25688,6 @@
       <c r="E227" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F227" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G227" s="6">
         <v>1</v>
       </c>
@@ -26302,9 +25720,6 @@
       <c r="E228" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F228" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G228" s="6">
         <v>1</v>
       </c>
@@ -26337,9 +25752,6 @@
       <c r="E229" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F229" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G229" s="6">
         <v>3</v>
       </c>
@@ -26372,9 +25784,6 @@
       <c r="E230" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F230" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G230" s="6">
         <v>3</v>
       </c>
@@ -26407,9 +25816,6 @@
       <c r="E231" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F231" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G231" s="6">
         <v>1</v>
       </c>
@@ -26445,9 +25851,6 @@
       <c r="E232" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F232" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G232" s="6">
         <v>3</v>
       </c>
@@ -26480,9 +25883,6 @@
       <c r="E233" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F233" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G233" s="6">
         <v>2</v>
       </c>
@@ -26515,9 +25915,6 @@
       <c r="E234" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F234" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G234" s="6">
         <v>1</v>
       </c>
@@ -26550,9 +25947,6 @@
       <c r="E235" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F235" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G235" s="6">
         <v>1</v>
       </c>
@@ -26585,9 +25979,6 @@
       <c r="E236" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F236" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G236" s="6">
         <v>3</v>
       </c>
@@ -26620,9 +26011,6 @@
       <c r="E237" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F237" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G237" s="6">
         <v>3</v>
       </c>
@@ -26655,9 +26043,6 @@
       <c r="E238" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F238" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="G238" s="6">
         <v>3</v>
       </c>
@@ -26690,9 +26075,6 @@
       <c r="E239" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F239" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G239" s="6">
         <v>3</v>
       </c>
@@ -26725,9 +26107,6 @@
       <c r="E240" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F240" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="G240" s="6">
         <v>3</v>
       </c>
@@ -26760,9 +26139,6 @@
       <c r="E241" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F241" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="G241" s="6">
         <v>3</v>
       </c>
@@ -26795,9 +26171,6 @@
       <c r="E242" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F242" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="G242" s="6">
         <v>3</v>
       </c>
@@ -26830,9 +26203,6 @@
       <c r="E243" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F243" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="G243" s="6">
         <v>3</v>
       </c>
@@ -26865,9 +26235,6 @@
       <c r="E244" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F244" s="6" t="s">
-        <v>312</v>
-      </c>
       <c r="G244" s="6">
         <v>3</v>
       </c>
@@ -26900,9 +26267,6 @@
       <c r="E245" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F245" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="G245" s="6">
         <v>3</v>
       </c>
@@ -26935,9 +26299,6 @@
       <c r="E246" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F246" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="G246" s="6">
         <v>1</v>
       </c>
@@ -26970,9 +26331,6 @@
       <c r="E247" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F247" s="6" t="s">
-        <v>313</v>
-      </c>
       <c r="G247" s="6">
         <v>3</v>
       </c>
@@ -27005,9 +26363,6 @@
       <c r="E248" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F248" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="G248" s="6">
         <v>3</v>
       </c>
@@ -27040,9 +26395,6 @@
       <c r="E249" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F249" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="G249" s="6">
         <v>1</v>
       </c>
@@ -27073,9 +26425,6 @@
         <v>15</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F250" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G250" s="6">

</xml_diff>

<commit_message>
REQ: only portal users are added to the portal (the other ones are skipped)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="15"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8518" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8532" uniqueCount="1135">
   <si>
     <t>SVN</t>
   </si>
@@ -3627,6 +3627,9 @@
   </si>
   <si>
     <t>Main menu (filter) has different style of tooltip</t>
+  </si>
+  <si>
+    <t>portal user</t>
   </si>
 </sst>
 </file>
@@ -27541,7 +27544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A508" workbookViewId="0">
+    <sheetView topLeftCell="A508" workbookViewId="0">
       <selection activeCell="N671" sqref="N671"/>
     </sheetView>
   </sheetViews>
@@ -51991,10 +51994,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -52005,7 +52008,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -52021,8 +52024,11 @@
       <c r="E1" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -52038,8 +52044,11 @@
       <c r="E2" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -52055,8 +52064,11 @@
       <c r="E3" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="26" t="s">
         <v>231</v>
       </c>
@@ -52070,8 +52082,11 @@
       <c r="E4" s="26" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="26" t="s">
         <v>241</v>
       </c>
@@ -52085,8 +52100,11 @@
       <c r="E5" s="26" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="26" t="s">
         <v>232</v>
       </c>
@@ -52100,8 +52118,11 @@
       <c r="E6" s="26" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="26" t="s">
         <v>233</v>
       </c>
@@ -52115,8 +52136,11 @@
       <c r="E7" s="26" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="26" t="s">
         <v>234</v>
       </c>
@@ -52130,8 +52154,11 @@
       <c r="E8" s="26" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="26" t="s">
         <v>235</v>
       </c>
@@ -52145,8 +52172,11 @@
       <c r="E9" s="26" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="26" t="s">
         <v>236</v>
       </c>
@@ -52160,8 +52190,11 @@
       <c r="E10" s="26" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="26" t="s">
         <v>237</v>
       </c>
@@ -52175,8 +52208,11 @@
       <c r="E11" s="26" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="26" t="s">
         <v>238</v>
       </c>
@@ -52190,8 +52226,11 @@
       <c r="E12" s="26" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="26" t="s">
         <v>239</v>
       </c>
@@ -52205,8 +52244,11 @@
       <c r="E13" s="26" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="26" t="s">
         <v>240</v>
       </c>
@@ -52219,6 +52261,9 @@
       </c>
       <c r="E14" s="26" t="s">
         <v>776</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REQ: improving project task data - requirements of sprint #6 have better descriptions + time when started / finished improved
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -27544,15 +27544,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P746"/>
   <sheetViews>
-    <sheetView topLeftCell="A508" workbookViewId="0">
-      <selection activeCell="N671" sqref="N671"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="O250" sqref="O250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="32" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="75.140625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="32" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="32" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="32" customWidth="1"/>
     <col min="6" max="8" width="17.42578125" style="32" customWidth="1"/>
@@ -30859,7 +30859,7 @@
         <v>4</v>
       </c>
       <c r="O98" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:15">
@@ -30925,7 +30925,7 @@
         <v>2</v>
       </c>
       <c r="O100" s="32">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:15">
@@ -35812,13 +35812,13 @@
         <v>418</v>
       </c>
       <c r="M250" s="32">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N250" s="32">
         <v>5</v>
       </c>
       <c r="O250" s="32">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="251" spans="1:15">
@@ -51996,7 +51996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
REQ: configure project not to send e-mail notifications (+ do not create tasks); also set RBLI assignees -> should be save (as no notifications are being sent)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" firstSheet="5" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8532" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8749" uniqueCount="1135">
   <si>
     <t>SVN</t>
   </si>
@@ -4264,7 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -20075,8 +20075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L336"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20149,7 +20149,7 @@
         <v>320</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>15</v>
+        <v>309</v>
       </c>
       <c r="G2" s="32">
         <v>4</v>
@@ -20183,6 +20183,9 @@
       <c r="E3" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F3" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G3" s="32">
         <v>6</v>
       </c>
@@ -20215,6 +20218,9 @@
       <c r="E4" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F4" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G4" s="32">
         <v>10</v>
       </c>
@@ -20247,6 +20253,9 @@
       <c r="E5" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F5" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G5" s="32">
         <v>6</v>
       </c>
@@ -20279,6 +20288,9 @@
       <c r="E6" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F6" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G6" s="32">
         <v>2</v>
       </c>
@@ -20311,6 +20323,9 @@
       <c r="E7" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F7" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G7" s="32">
         <v>8</v>
       </c>
@@ -20343,6 +20358,9 @@
       <c r="E8" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F8" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G8" s="32">
         <v>6</v>
       </c>
@@ -20375,6 +20393,9 @@
       <c r="E9" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F9" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G9" s="32">
         <v>8</v>
       </c>
@@ -20407,6 +20428,9 @@
       <c r="E10" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F10" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G10" s="32">
         <v>2</v>
       </c>
@@ -20439,6 +20463,9 @@
       <c r="E11" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F11" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G11" s="32">
         <v>4</v>
       </c>
@@ -20471,6 +20498,9 @@
       <c r="E12" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F12" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G12" s="32">
         <v>2</v>
       </c>
@@ -20503,6 +20533,9 @@
       <c r="E13" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F13" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G13" s="32">
         <v>6</v>
       </c>
@@ -20538,6 +20571,9 @@
       <c r="E14" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F14" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G14" s="32">
         <v>8</v>
       </c>
@@ -20570,6 +20606,9 @@
       <c r="E15" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F15" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G15" s="32">
         <v>6</v>
       </c>
@@ -20602,6 +20641,9 @@
       <c r="E16" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F16" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G16" s="32">
         <v>2</v>
       </c>
@@ -20634,6 +20676,9 @@
       <c r="E17" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F17" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G17" s="32">
         <v>2</v>
       </c>
@@ -20666,6 +20711,9 @@
       <c r="E18" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F18" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G18" s="32">
         <v>6</v>
       </c>
@@ -20698,6 +20746,9 @@
       <c r="E19" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F19" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G19" s="32">
         <v>2</v>
       </c>
@@ -20730,6 +20781,9 @@
       <c r="E20" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F20" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G20" s="32">
         <v>2</v>
       </c>
@@ -20762,6 +20816,9 @@
       <c r="E21" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F21" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G21" s="32">
         <v>2</v>
       </c>
@@ -20794,6 +20851,9 @@
       <c r="E22" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F22" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G22" s="32">
         <v>2</v>
       </c>
@@ -20826,6 +20886,9 @@
       <c r="E23" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F23" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G23" s="32">
         <v>6</v>
       </c>
@@ -20858,6 +20921,9 @@
       <c r="E24" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F24" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G24" s="32">
         <v>2</v>
       </c>
@@ -20890,6 +20956,9 @@
       <c r="E25" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F25" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G25" s="32">
         <v>2</v>
       </c>
@@ -20925,6 +20994,9 @@
       <c r="E26" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F26" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G26" s="32">
         <v>2</v>
       </c>
@@ -20957,6 +21029,9 @@
       <c r="E27" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F27" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G27" s="32">
         <v>6</v>
       </c>
@@ -20989,6 +21064,9 @@
       <c r="E28" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F28" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G28" s="32">
         <v>6</v>
       </c>
@@ -21021,6 +21099,9 @@
       <c r="E29" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F29" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G29" s="32">
         <v>2</v>
       </c>
@@ -21053,6 +21134,9 @@
       <c r="E30" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F30" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G30" s="32">
         <v>8</v>
       </c>
@@ -21085,6 +21169,9 @@
       <c r="E31" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F31" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G31" s="32">
         <v>2</v>
       </c>
@@ -21117,6 +21204,9 @@
       <c r="E32" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F32" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G32" s="32">
         <v>6</v>
       </c>
@@ -21149,6 +21239,9 @@
       <c r="E33" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F33" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G33" s="32">
         <v>2</v>
       </c>
@@ -21181,6 +21274,9 @@
       <c r="E34" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F34" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G34" s="32">
         <v>2</v>
       </c>
@@ -21213,6 +21309,9 @@
       <c r="E35" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F35" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G35" s="32">
         <v>6</v>
       </c>
@@ -21245,6 +21344,9 @@
       <c r="E36" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F36" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G36" s="32">
         <v>8</v>
       </c>
@@ -21277,6 +21379,9 @@
       <c r="E37" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F37" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G37" s="32">
         <v>2</v>
       </c>
@@ -21309,6 +21414,9 @@
       <c r="E38" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F38" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G38" s="32">
         <v>4</v>
       </c>
@@ -21341,6 +21449,9 @@
       <c r="E39" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F39" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G39" s="32">
         <v>8</v>
       </c>
@@ -21373,6 +21484,9 @@
       <c r="E40" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F40" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G40" s="32">
         <v>2</v>
       </c>
@@ -21405,6 +21519,9 @@
       <c r="E41" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F41" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G41" s="32">
         <v>6</v>
       </c>
@@ -21437,6 +21554,9 @@
       <c r="E42" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F42" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G42" s="32">
         <v>2</v>
       </c>
@@ -21469,6 +21589,9 @@
       <c r="E43" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F43" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G43" s="32">
         <v>2</v>
       </c>
@@ -21501,6 +21624,9 @@
       <c r="E44" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F44" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G44" s="32">
         <v>2</v>
       </c>
@@ -21533,6 +21659,9 @@
       <c r="E45" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F45" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G45" s="32">
         <v>8</v>
       </c>
@@ -21565,6 +21694,9 @@
       <c r="E46" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F46" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G46" s="32">
         <v>8</v>
       </c>
@@ -21597,6 +21729,9 @@
       <c r="E47" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F47" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G47" s="32">
         <v>2</v>
       </c>
@@ -21629,6 +21764,9 @@
       <c r="E48" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F48" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G48" s="32">
         <v>8</v>
       </c>
@@ -21661,6 +21799,9 @@
       <c r="E49" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F49" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G49" s="32">
         <v>6</v>
       </c>
@@ -21693,6 +21834,9 @@
       <c r="E50" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F50" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G50" s="32">
         <v>4</v>
       </c>
@@ -21725,6 +21869,9 @@
       <c r="E51" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F51" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G51" s="32">
         <v>2</v>
       </c>
@@ -21757,6 +21904,9 @@
       <c r="E52" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F52" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G52" s="32">
         <v>6</v>
       </c>
@@ -21789,6 +21939,9 @@
       <c r="E53" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F53" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G53" s="32">
         <v>6</v>
       </c>
@@ -21821,6 +21974,9 @@
       <c r="E54" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F54" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G54" s="32">
         <v>6</v>
       </c>
@@ -21853,6 +22009,9 @@
       <c r="E55" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F55" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G55" s="32">
         <v>2</v>
       </c>
@@ -21885,6 +22044,9 @@
       <c r="E56" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F56" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G56" s="32">
         <v>2</v>
       </c>
@@ -21917,6 +22079,9 @@
       <c r="E57" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F57" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G57" s="32">
         <v>6</v>
       </c>
@@ -21949,6 +22114,9 @@
       <c r="E58" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F58" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G58" s="32">
         <v>2</v>
       </c>
@@ -21981,6 +22149,9 @@
       <c r="E59" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F59" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G59" s="32">
         <v>2</v>
       </c>
@@ -22013,6 +22184,9 @@
       <c r="E60" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F60" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G60" s="32">
         <v>4</v>
       </c>
@@ -22045,6 +22219,9 @@
       <c r="E61" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F61" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G61" s="32">
         <v>2</v>
       </c>
@@ -22077,6 +22254,9 @@
       <c r="E62" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F62" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G62" s="32">
         <v>6</v>
       </c>
@@ -22109,6 +22289,9 @@
       <c r="E63" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F63" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G63" s="32">
         <v>4</v>
       </c>
@@ -22141,6 +22324,9 @@
       <c r="E64" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F64" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G64" s="32">
         <v>6</v>
       </c>
@@ -22173,6 +22359,9 @@
       <c r="E65" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F65" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G65" s="32">
         <v>2</v>
       </c>
@@ -22205,6 +22394,9 @@
       <c r="E66" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F66" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G66" s="32">
         <v>8</v>
       </c>
@@ -22237,6 +22429,9 @@
       <c r="E67" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F67" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G67" s="32">
         <v>2</v>
       </c>
@@ -22269,6 +22464,9 @@
       <c r="E68" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F68" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G68" s="32">
         <v>2</v>
       </c>
@@ -22301,6 +22499,9 @@
       <c r="E69" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F69" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G69" s="32">
         <v>2</v>
       </c>
@@ -22333,6 +22534,9 @@
       <c r="E70" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F70" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G70" s="32">
         <v>6</v>
       </c>
@@ -22365,6 +22569,9 @@
       <c r="E71" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F71" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G71" s="32">
         <v>6</v>
       </c>
@@ -22397,6 +22604,9 @@
       <c r="E72" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F72" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G72" s="32">
         <v>6</v>
       </c>
@@ -22429,6 +22639,9 @@
       <c r="E73" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F73" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G73" s="32">
         <v>2</v>
       </c>
@@ -22461,6 +22674,9 @@
       <c r="E74" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F74" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G74" s="32">
         <v>2</v>
       </c>
@@ -22493,6 +22709,9 @@
       <c r="E75" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F75" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G75" s="32">
         <v>6</v>
       </c>
@@ -22525,6 +22744,9 @@
       <c r="E76" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F76" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G76" s="32">
         <v>2</v>
       </c>
@@ -22557,6 +22779,9 @@
       <c r="E77" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F77" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G77" s="32">
         <v>2</v>
       </c>
@@ -22589,6 +22814,9 @@
       <c r="E78" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F78" s="32" t="s">
+        <v>319</v>
+      </c>
       <c r="G78" s="32">
         <v>2</v>
       </c>
@@ -22621,6 +22849,9 @@
       <c r="E79" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F79" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="G79" s="32">
         <v>2</v>
       </c>
@@ -22653,6 +22884,9 @@
       <c r="E80" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F80" s="32" t="s">
+        <v>310</v>
+      </c>
       <c r="G80" s="32">
         <v>6</v>
       </c>
@@ -22685,6 +22919,9 @@
       <c r="E81" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F81" s="32" t="s">
+        <v>317</v>
+      </c>
       <c r="G81" s="32">
         <v>2</v>
       </c>
@@ -22717,6 +22954,9 @@
       <c r="E82" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F82" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="G82" s="32">
         <v>12</v>
       </c>
@@ -22749,6 +22989,9 @@
       <c r="E83" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F83" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G83" s="32">
         <v>2</v>
       </c>
@@ -22781,6 +23024,9 @@
       <c r="E84" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F84" s="32" t="s">
+        <v>318</v>
+      </c>
       <c r="G84" s="32">
         <v>2</v>
       </c>
@@ -22813,6 +23059,9 @@
       <c r="E85" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F85" s="32" t="s">
+        <v>315</v>
+      </c>
       <c r="G85" s="32">
         <v>6</v>
       </c>
@@ -22845,6 +23094,9 @@
       <c r="E86" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F86" s="32" t="s">
+        <v>309</v>
+      </c>
       <c r="G86" s="32">
         <v>4</v>
       </c>
@@ -22877,6 +23129,9 @@
       <c r="E87" s="32" t="s">
         <v>322</v>
       </c>
+      <c r="F87" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="G87" s="32">
         <v>6</v>
       </c>
@@ -22909,6 +23164,9 @@
       <c r="E88" s="32" t="s">
         <v>321</v>
       </c>
+      <c r="F88" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="G88" s="32">
         <v>2</v>
       </c>
@@ -22941,6 +23199,9 @@
       <c r="E89" s="32" t="s">
         <v>320</v>
       </c>
+      <c r="F89" s="32" t="s">
+        <v>311</v>
+      </c>
       <c r="G89" s="32">
         <v>2</v>
       </c>
@@ -22973,6 +23234,9 @@
       <c r="E90" s="32" t="s">
         <v>15</v>
       </c>
+      <c r="F90" s="32" t="s">
+        <v>15</v>
+      </c>
       <c r="G90" s="32">
         <v>6</v>
       </c>
@@ -23372,6 +23636,9 @@
       <c r="E122" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F122" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G122" s="32">
         <v>3</v>
       </c>
@@ -23404,6 +23671,9 @@
       <c r="E123" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F123" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G123" s="32">
         <v>5</v>
       </c>
@@ -23436,6 +23706,9 @@
       <c r="E124" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F124" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G124" s="32">
         <v>7</v>
       </c>
@@ -23468,6 +23741,9 @@
       <c r="E125" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F125" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G125" s="6">
         <v>3</v>
       </c>
@@ -23500,6 +23776,9 @@
       <c r="E126" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F126" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G126" s="6">
         <v>1</v>
       </c>
@@ -23532,6 +23811,9 @@
       <c r="E127" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F127" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G127" s="6">
         <v>5</v>
       </c>
@@ -23564,6 +23846,9 @@
       <c r="E128" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F128" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G128" s="6">
         <v>3</v>
       </c>
@@ -23596,6 +23881,9 @@
       <c r="E129" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F129" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G129" s="6">
         <v>5</v>
       </c>
@@ -23628,6 +23916,9 @@
       <c r="E130" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F130" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G130" s="6">
         <v>1</v>
       </c>
@@ -23660,6 +23951,9 @@
       <c r="E131" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F131" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G131" s="6">
         <v>3</v>
       </c>
@@ -23692,6 +23986,9 @@
       <c r="E132" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F132" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G132" s="6">
         <v>3</v>
       </c>
@@ -23724,6 +24021,9 @@
       <c r="E133" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F133" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G133" s="6">
         <v>3</v>
       </c>
@@ -23756,6 +24056,9 @@
       <c r="E134" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F134" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G134" s="6">
         <v>3</v>
       </c>
@@ -23788,6 +24091,9 @@
       <c r="E135" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F135" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G135" s="6">
         <v>3</v>
       </c>
@@ -23820,6 +24126,9 @@
       <c r="E136" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F136" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G136" s="6">
         <v>3</v>
       </c>
@@ -23852,6 +24161,9 @@
       <c r="E137" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F137" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G137" s="6">
         <v>3</v>
       </c>
@@ -23884,6 +24196,9 @@
       <c r="E138" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F138" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G138" s="6">
         <v>1</v>
       </c>
@@ -23916,6 +24231,9 @@
       <c r="E139" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F139" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G139" s="6">
         <v>3</v>
       </c>
@@ -23948,6 +24266,9 @@
       <c r="E140" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F140" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G140" s="6">
         <v>3</v>
       </c>
@@ -23980,6 +24301,9 @@
       <c r="E141" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F141" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G141" s="6">
         <v>1</v>
       </c>
@@ -24012,6 +24336,9 @@
       <c r="E142" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F142" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G142" s="6">
         <v>1</v>
       </c>
@@ -24044,6 +24371,9 @@
       <c r="E143" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F143" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G143" s="6">
         <v>2</v>
       </c>
@@ -24076,6 +24406,9 @@
       <c r="E144" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F144" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G144" s="6">
         <v>3</v>
       </c>
@@ -24108,6 +24441,9 @@
       <c r="E145" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F145" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G145" s="6">
         <v>3</v>
       </c>
@@ -24140,6 +24476,9 @@
       <c r="E146" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F146" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G146" s="6">
         <v>2</v>
       </c>
@@ -24172,6 +24511,9 @@
       <c r="E147" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F147" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G147" s="6">
         <v>3</v>
       </c>
@@ -24204,6 +24546,9 @@
       <c r="E148" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F148" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G148" s="6">
         <v>3</v>
       </c>
@@ -24236,6 +24581,9 @@
       <c r="E149" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F149" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G149" s="6">
         <v>3</v>
       </c>
@@ -24268,6 +24616,9 @@
       <c r="E150" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F150" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G150" s="6">
         <v>2</v>
       </c>
@@ -24300,6 +24651,9 @@
       <c r="E151" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F151" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G151" s="6">
         <v>2</v>
       </c>
@@ -24332,6 +24686,9 @@
       <c r="E152" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F152" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G152" s="6">
         <v>2</v>
       </c>
@@ -24364,6 +24721,9 @@
       <c r="E153" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F153" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G153" s="6">
         <v>2</v>
       </c>
@@ -24396,6 +24756,9 @@
       <c r="E154" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F154" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G154" s="6">
         <v>2</v>
       </c>
@@ -24428,6 +24791,9 @@
       <c r="E155" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F155" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G155" s="6">
         <v>1</v>
       </c>
@@ -24460,6 +24826,9 @@
       <c r="E156" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F156" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G156" s="6">
         <v>1</v>
       </c>
@@ -24492,6 +24861,9 @@
       <c r="E157" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F157" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G157" s="6">
         <v>5</v>
       </c>
@@ -24524,6 +24896,9 @@
       <c r="E158" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F158" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G158" s="6">
         <v>3</v>
       </c>
@@ -24559,6 +24934,9 @@
       <c r="E159" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F159" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G159" s="6">
         <v>1</v>
       </c>
@@ -24591,6 +24969,9 @@
       <c r="E160" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F160" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G160" s="6">
         <v>3</v>
       </c>
@@ -24623,6 +25004,9 @@
       <c r="E161" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F161" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G161" s="6">
         <v>2</v>
       </c>
@@ -24655,6 +25039,9 @@
       <c r="E162" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F162" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G162" s="6">
         <v>1</v>
       </c>
@@ -24687,6 +25074,9 @@
       <c r="E163" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F163" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G163" s="6">
         <v>1</v>
       </c>
@@ -24719,6 +25109,9 @@
       <c r="E164" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F164" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G164" s="6">
         <v>3</v>
       </c>
@@ -24751,6 +25144,9 @@
       <c r="E165" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F165" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G165" s="6">
         <v>3</v>
       </c>
@@ -24783,6 +25179,9 @@
       <c r="E166" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F166" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G166" s="6">
         <v>3</v>
       </c>
@@ -24815,6 +25214,9 @@
       <c r="E167" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F167" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G167" s="6">
         <v>3</v>
       </c>
@@ -24847,6 +25249,9 @@
       <c r="E168" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F168" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G168" s="6">
         <v>3</v>
       </c>
@@ -24879,6 +25284,9 @@
       <c r="E169" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F169" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G169" s="6">
         <v>3</v>
       </c>
@@ -24911,6 +25319,9 @@
       <c r="E170" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F170" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G170" s="6">
         <v>3</v>
       </c>
@@ -24943,6 +25354,9 @@
       <c r="E171" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F171" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G171" s="6">
         <v>3</v>
       </c>
@@ -24975,6 +25389,9 @@
       <c r="E172" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F172" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G172" s="6">
         <v>3</v>
       </c>
@@ -25007,6 +25424,9 @@
       <c r="E173" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F173" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G173" s="6">
         <v>3</v>
       </c>
@@ -25039,6 +25459,9 @@
       <c r="E174" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F174" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G174" s="6">
         <v>2</v>
       </c>
@@ -25071,6 +25494,9 @@
       <c r="E175" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F175" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G175" s="6">
         <v>3</v>
       </c>
@@ -25103,6 +25529,9 @@
       <c r="E176" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F176" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G176" s="6">
         <v>3</v>
       </c>
@@ -25135,6 +25564,9 @@
       <c r="E177" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F177" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G177" s="6">
         <v>1</v>
       </c>
@@ -25167,6 +25599,9 @@
       <c r="E178" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F178" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G178" s="6">
         <v>1</v>
       </c>
@@ -25199,6 +25634,9 @@
       <c r="E179" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F179" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G179" s="6">
         <v>1</v>
       </c>
@@ -25231,6 +25669,9 @@
       <c r="E180" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F180" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G180" s="6">
         <v>3</v>
       </c>
@@ -25263,6 +25704,9 @@
       <c r="E181" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F181" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G181" s="6">
         <v>3</v>
       </c>
@@ -25295,6 +25739,9 @@
       <c r="E182" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F182" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G182" s="6">
         <v>3</v>
       </c>
@@ -25327,6 +25774,9 @@
       <c r="E183" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F183" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G183" s="6">
         <v>3</v>
       </c>
@@ -25359,6 +25809,9 @@
       <c r="E184" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F184" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G184" s="6">
         <v>3</v>
       </c>
@@ -25391,6 +25844,9 @@
       <c r="E185" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F185" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G185" s="6">
         <v>3</v>
       </c>
@@ -25423,6 +25879,9 @@
       <c r="E186" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F186" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G186" s="6">
         <v>4</v>
       </c>
@@ -25455,6 +25914,9 @@
       <c r="E187" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F187" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G187" s="6">
         <v>2</v>
       </c>
@@ -25487,6 +25949,9 @@
       <c r="E188" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F188" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G188" s="6">
         <v>3</v>
       </c>
@@ -25519,6 +25984,9 @@
       <c r="E189" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F189" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G189" s="6">
         <v>3</v>
       </c>
@@ -25551,6 +26019,9 @@
       <c r="E190" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F190" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G190" s="6">
         <v>3</v>
       </c>
@@ -25583,6 +26054,9 @@
       <c r="E191" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F191" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G191" s="6">
         <v>1</v>
       </c>
@@ -25615,6 +26089,9 @@
       <c r="E192" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F192" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G192" s="6">
         <v>1</v>
       </c>
@@ -25647,6 +26124,9 @@
       <c r="E193" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F193" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G193" s="6">
         <v>3</v>
       </c>
@@ -25682,6 +26162,9 @@
       <c r="E194" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F194" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G194" s="6">
         <v>3</v>
       </c>
@@ -25714,6 +26197,9 @@
       <c r="E195" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F195" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G195" s="6">
         <v>1</v>
       </c>
@@ -25746,6 +26232,9 @@
       <c r="E196" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F196" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G196" s="6">
         <v>3</v>
       </c>
@@ -25778,6 +26267,9 @@
       <c r="E197" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F197" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G197" s="6">
         <v>2</v>
       </c>
@@ -25810,6 +26302,9 @@
       <c r="E198" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F198" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G198" s="6">
         <v>1</v>
       </c>
@@ -25842,6 +26337,9 @@
       <c r="E199" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F199" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G199" s="6">
         <v>1</v>
       </c>
@@ -25874,6 +26372,9 @@
       <c r="E200" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F200" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G200" s="6">
         <v>3</v>
       </c>
@@ -25906,6 +26407,9 @@
       <c r="E201" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F201" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G201" s="6">
         <v>3</v>
       </c>
@@ -25938,6 +26442,9 @@
       <c r="E202" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F202" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G202" s="6">
         <v>3</v>
       </c>
@@ -25970,6 +26477,9 @@
       <c r="E203" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F203" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G203" s="6">
         <v>3</v>
       </c>
@@ -26002,6 +26512,9 @@
       <c r="E204" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F204" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G204" s="6">
         <v>3</v>
       </c>
@@ -26034,6 +26547,9 @@
       <c r="E205" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F205" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G205" s="6">
         <v>3</v>
       </c>
@@ -26066,6 +26582,9 @@
       <c r="E206" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F206" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G206" s="6">
         <v>3</v>
       </c>
@@ -26098,6 +26617,9 @@
       <c r="E207" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F207" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G207" s="6">
         <v>3</v>
       </c>
@@ -26130,6 +26652,9 @@
       <c r="E208" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F208" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G208" s="6">
         <v>3</v>
       </c>
@@ -26162,6 +26687,9 @@
       <c r="E209" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F209" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G209" s="6">
         <v>3</v>
       </c>
@@ -26194,6 +26722,9 @@
       <c r="E210" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F210" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G210" s="6">
         <v>2</v>
       </c>
@@ -26226,6 +26757,9 @@
       <c r="E211" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F211" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G211" s="6">
         <v>3</v>
       </c>
@@ -26258,6 +26792,9 @@
       <c r="E212" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F212" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G212" s="6">
         <v>3</v>
       </c>
@@ -26290,6 +26827,9 @@
       <c r="E213" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F213" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G213" s="6">
         <v>1</v>
       </c>
@@ -26325,6 +26865,9 @@
       <c r="E214" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F214" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G214" s="6">
         <v>2</v>
       </c>
@@ -26357,6 +26900,9 @@
       <c r="E215" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F215" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G215" s="6">
         <v>2</v>
       </c>
@@ -26389,6 +26935,9 @@
       <c r="E216" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F216" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G216" s="6">
         <v>3</v>
       </c>
@@ -26421,6 +26970,9 @@
       <c r="E217" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F217" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G217" s="6">
         <v>3</v>
       </c>
@@ -26453,6 +27005,9 @@
       <c r="E218" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F218" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G218" s="6">
         <v>2</v>
       </c>
@@ -26485,6 +27040,9 @@
       <c r="E219" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F219" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G219" s="6">
         <v>3</v>
       </c>
@@ -26517,6 +27075,9 @@
       <c r="E220" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F220" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G220" s="6">
         <v>3</v>
       </c>
@@ -26549,6 +27110,9 @@
       <c r="E221" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F221" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G221" s="6">
         <v>3</v>
       </c>
@@ -26581,6 +27145,9 @@
       <c r="E222" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F222" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G222" s="6">
         <v>5</v>
       </c>
@@ -26613,6 +27180,9 @@
       <c r="E223" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F223" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G223" s="6">
         <v>4</v>
       </c>
@@ -26645,6 +27215,9 @@
       <c r="E224" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F224" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G224" s="6">
         <v>3</v>
       </c>
@@ -26677,6 +27250,9 @@
       <c r="E225" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F225" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G225" s="6">
         <v>3</v>
       </c>
@@ -26709,6 +27285,9 @@
       <c r="E226" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F226" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G226" s="6">
         <v>3</v>
       </c>
@@ -26741,6 +27320,9 @@
       <c r="E227" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F227" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G227" s="6">
         <v>1</v>
       </c>
@@ -26773,6 +27355,9 @@
       <c r="E228" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F228" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G228" s="6">
         <v>1</v>
       </c>
@@ -26805,6 +27390,9 @@
       <c r="E229" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F229" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G229" s="6">
         <v>3</v>
       </c>
@@ -26837,6 +27425,9 @@
       <c r="E230" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F230" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G230" s="6">
         <v>3</v>
       </c>
@@ -26869,6 +27460,9 @@
       <c r="E231" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F231" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G231" s="6">
         <v>1</v>
       </c>
@@ -26904,6 +27498,9 @@
       <c r="E232" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F232" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G232" s="6">
         <v>3</v>
       </c>
@@ -26936,6 +27533,9 @@
       <c r="E233" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F233" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G233" s="6">
         <v>2</v>
       </c>
@@ -26968,6 +27568,9 @@
       <c r="E234" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F234" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G234" s="6">
         <v>1</v>
       </c>
@@ -27000,6 +27603,9 @@
       <c r="E235" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F235" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G235" s="6">
         <v>1</v>
       </c>
@@ -27032,6 +27638,9 @@
       <c r="E236" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F236" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G236" s="6">
         <v>3</v>
       </c>
@@ -27064,6 +27673,9 @@
       <c r="E237" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F237" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G237" s="6">
         <v>3</v>
       </c>
@@ -27096,6 +27708,9 @@
       <c r="E238" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F238" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G238" s="6">
         <v>3</v>
       </c>
@@ -27128,6 +27743,9 @@
       <c r="E239" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F239" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G239" s="6">
         <v>3</v>
       </c>
@@ -27160,6 +27778,9 @@
       <c r="E240" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F240" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G240" s="6">
         <v>3</v>
       </c>
@@ -27192,6 +27813,9 @@
       <c r="E241" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F241" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="G241" s="6">
         <v>3</v>
       </c>
@@ -27224,6 +27848,9 @@
       <c r="E242" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F242" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="G242" s="6">
         <v>3</v>
       </c>
@@ -27256,6 +27883,9 @@
       <c r="E243" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F243" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="G243" s="6">
         <v>3</v>
       </c>
@@ -27288,6 +27918,9 @@
       <c r="E244" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F244" s="6" t="s">
+        <v>312</v>
+      </c>
       <c r="G244" s="6">
         <v>3</v>
       </c>
@@ -27320,6 +27953,9 @@
       <c r="E245" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F245" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="G245" s="6">
         <v>3</v>
       </c>
@@ -27352,6 +27988,9 @@
       <c r="E246" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F246" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="G246" s="6">
         <v>1</v>
       </c>
@@ -27384,6 +28023,9 @@
       <c r="E247" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F247" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="G247" s="6">
         <v>3</v>
       </c>
@@ -27416,6 +28058,9 @@
       <c r="E248" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="F248" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="G248" s="6">
         <v>3</v>
       </c>
@@ -27448,6 +28093,9 @@
       <c r="E249" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="F249" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="G249" s="6">
         <v>1</v>
       </c>
@@ -27478,6 +28126,9 @@
         <v>15</v>
       </c>
       <c r="E250" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F250" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G250" s="6">

</xml_diff>

<commit_message>
REQ: support for setting user phone number (from Excel file)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="18"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'release-backlog-item'!$F$1:$F$336</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Settings!$B$4:$C$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateCount="1"/>
 </workbook>
 </file>
 
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8750" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8751" uniqueCount="1136">
   <si>
     <t>SVN</t>
   </si>
@@ -3630,6 +3630,9 @@
   </si>
   <si>
     <t>#products-id</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
 </sst>
 </file>
@@ -5394,7 +5397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -52741,10 +52744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -52753,9 +52756,10 @@
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -52771,11 +52775,14 @@
       <c r="E1" t="s">
         <v>779</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="32" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G1" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -52791,11 +52798,14 @@
       <c r="E2" t="s">
         <v>776</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="32">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -52811,11 +52821,11 @@
       <c r="E3" t="s">
         <v>777</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="26" t="s">
         <v>231</v>
       </c>
@@ -52829,11 +52839,11 @@
       <c r="E4" s="26" t="s">
         <v>753</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="26" t="s">
         <v>241</v>
       </c>
@@ -52847,11 +52857,11 @@
       <c r="E5" s="26" t="s">
         <v>756</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="G5" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="26" t="s">
         <v>232</v>
       </c>
@@ -52865,11 +52875,11 @@
       <c r="E6" s="26" t="s">
         <v>758</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="G6" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="26" t="s">
         <v>233</v>
       </c>
@@ -52883,11 +52893,11 @@
       <c r="E7" s="26" t="s">
         <v>760</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="G7" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="26" t="s">
         <v>234</v>
       </c>
@@ -52901,11 +52911,11 @@
       <c r="E8" s="26" t="s">
         <v>762</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="G8" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="26" t="s">
         <v>235</v>
       </c>
@@ -52919,11 +52929,11 @@
       <c r="E9" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="G9" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="26" t="s">
         <v>236</v>
       </c>
@@ -52937,11 +52947,11 @@
       <c r="E10" s="26" t="s">
         <v>766</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="G10" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="26" t="s">
         <v>237</v>
       </c>
@@ -52955,11 +52965,11 @@
       <c r="E11" s="26" t="s">
         <v>768</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="G11" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="26" t="s">
         <v>238</v>
       </c>
@@ -52973,11 +52983,11 @@
       <c r="E12" s="26" t="s">
         <v>770</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="G12" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="26" t="s">
         <v>239</v>
       </c>
@@ -52991,11 +53001,11 @@
       <c r="E13" s="26" t="s">
         <v>772</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="G13" s="32" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="26" t="s">
         <v>240</v>
       </c>
@@ -53009,7 +53019,7 @@
       <c r="E14" s="26" t="s">
         <v>774</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="G14" s="32" t="s">
         <v>338</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REQ: Hudson service name can be set in settings now (support for Jenkins)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8751" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8753" uniqueCount="1137">
   <si>
     <t>SVN</t>
   </si>
@@ -3633,6 +3633,9 @@
   </si>
   <si>
     <t>phone</t>
+  </si>
+  <si>
+    <t>Hudson Service Name</t>
   </si>
 </sst>
 </file>
@@ -8044,8 +8047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8322,6 +8325,14 @@
       </c>
       <c r="C28" s="31" t="s">
         <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="29" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -52746,7 +52757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ENH: moving BuildServerName property to Settings (removing hack and BuildServerHandler)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8745" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8746" uniqueCount="1135">
   <si>
     <t>SVN</t>
   </si>
@@ -3627,6 +3627,9 @@
   </si>
   <si>
     <t>Use if requirements have been already pre-generated</t>
+  </si>
+  <si>
+    <t>BuildServerName</t>
   </si>
 </sst>
 </file>
@@ -4261,7 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -8042,8 +8045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:C23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8324,8 +8327,12 @@
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="29" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="7"/>
@@ -54695,7 +54702,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54754,8 +54761,9 @@
       <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
+      <c r="E2" t="str">
+        <f>Settings!$C$30</f>
+        <v>Hudson</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>Settings!$C$13</f>

</xml_diff>

<commit_message>
REQ: support for fomulas - cells can reference other cells + Settings sheet can be overwritten by settings.properties file first
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8746" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8744" uniqueCount="1135">
   <si>
     <t>SVN</t>
   </si>
@@ -4264,7 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -8045,8 +8045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54796,7 +54796,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54847,11 +54847,13 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
-        <v>918</v>
-      </c>
-      <c r="D2" t="s">
-        <v>918</v>
+      <c r="C2" t="str">
+        <f>Settings!$C$14</f>
+        <v>MediaStore</v>
+      </c>
+      <c r="D2" t="str">
+        <f>Settings!$C$14</f>
+        <v>MediaStore</v>
       </c>
       <c r="E2" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
ENH: moving BranchPath property to settings (hard-coded string)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8744" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8745" uniqueCount="1136">
   <si>
     <t>SVN</t>
   </si>
@@ -3630,6 +3630,9 @@
   </si>
   <si>
     <t>BuildServerName</t>
+  </si>
+  <si>
+    <t>BranchPath</t>
   </si>
 </sst>
 </file>
@@ -4386,7 +4389,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4421,8 +4424,9 @@
       <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
-        <v>317</v>
+      <c r="D2" t="str">
+        <f>Settings!$C$31</f>
+        <v>/trunk</v>
       </c>
       <c r="E2" t="s">
         <v>53</v>
@@ -8046,7 +8050,7 @@
   <dimension ref="B1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8335,8 +8339,12 @@
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="29" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="7"/>

</xml_diff>

<commit_message>
REQ: keep release when refreshing data (do not delete it but reuse)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8745" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8748" uniqueCount="1138">
   <si>
     <t>SVN</t>
   </si>
@@ -3633,6 +3633,12 @@
   </si>
   <si>
     <t>BranchPath</t>
+  </si>
+  <si>
+    <t>KeepRelease</t>
+  </si>
+  <si>
+    <t>ReleaseName</t>
   </si>
 </sst>
 </file>
@@ -8050,7 +8056,7 @@
   <dimension ref="B1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8347,12 +8353,20 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="29" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="B33" s="29" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="7"/>
@@ -54377,7 +54391,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54436,8 +54450,9 @@
       <c r="F2" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>916</v>
+      <c r="G2" s="5" t="str">
+        <f>Settings!$C$33</f>
+        <v>HP Media Store 2.0</v>
       </c>
       <c r="H2" t="s">
         <v>917</v>

</xml_diff>

<commit_message>
BUG: the number of revisions in SVN/uimafit is 923; increasing the number of revisions in the very last build from 30 into 32
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="22680" windowHeight="9030" tabRatio="954" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -8055,7 +8055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -53071,8 +53071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54219,7 +54219,7 @@
         <v>86400000</v>
       </c>
       <c r="I60">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J60">
         <f t="shared" si="2"/>

</xml_diff>